<commit_message>
Fabric + DepencyInhection + logger
</commit_message>
<xml_diff>
--- a/bot_unemployment_scrap/report/final_report.xlsx
+++ b/bot_unemployment_scrap/report/final_report.xlsx
@@ -582,14 +582,14 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="C7" t="n">
         <v>92.8</v>
       </c>
-      <c r="C7" t="n">
-        <v>91.7</v>
-      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2022-05</t>
+          <t>2022-06</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -651,14 +651,14 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>81.2</v>
+      </c>
+      <c r="C10" t="n">
         <v>81</v>
       </c>
-      <c r="C10" t="n">
-        <v>81.59999999999999</v>
-      </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -674,14 +674,14 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>79.3</v>
+      </c>
+      <c r="C11" t="n">
         <v>80.40000000000001</v>
       </c>
-      <c r="C11" t="n">
-        <v>79.40000000000001</v>
-      </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -720,14 +720,14 @@
         </is>
       </c>
       <c r="B13" t="n">
+        <v>77</v>
+      </c>
+      <c r="C13" t="n">
         <v>76.90000000000001</v>
       </c>
-      <c r="C13" t="n">
-        <v>76.7</v>
-      </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -743,14 +743,14 @@
         </is>
       </c>
       <c r="B14" t="n">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="C14" t="n">
         <v>76.7</v>
       </c>
-      <c r="C14" t="n">
-        <v>75.09999999999999</v>
-      </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -785,14 +785,14 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>República Tcheca</t>
+          <t>Bolívia</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>75.3</v>
+        <v>75.2</v>
       </c>
       <c r="C16" t="n">
-        <v>75</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -808,18 +808,18 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Bolívia</t>
+          <t>República Tcheca</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>75.2</v>
+        <v>75</v>
       </c>
       <c r="C17" t="n">
-        <v>73.59999999999999</v>
+        <v>75.3</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -858,14 +858,14 @@
         </is>
       </c>
       <c r="B19" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="C19" t="n">
         <v>73.5</v>
       </c>
-      <c r="C19" t="n">
-        <v>74</v>
-      </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -877,18 +877,18 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Lituânia</t>
+          <t>Irlanda</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>73.2</v>
+        <v>72.8</v>
       </c>
       <c r="C20" t="n">
-        <v>73.2</v>
+        <v>73</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -900,14 +900,14 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Irlanda</t>
+          <t>Lituânia</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>72.8</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>73</v>
+        <v>73.2</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -927,14 +927,14 @@
         </is>
       </c>
       <c r="B22" t="n">
+        <v>72.5</v>
+      </c>
+      <c r="C22" t="n">
         <v>72.40000000000001</v>
       </c>
-      <c r="C22" t="n">
-        <v>73.40000000000001</v>
-      </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -950,14 +950,14 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>72.3</v>
+        <v>72</v>
       </c>
       <c r="C23" t="n">
         <v>72.3</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -980,7 +980,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -992,18 +992,18 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Eslováquia</t>
+          <t>Luxemburgo</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>70.8</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="C25" t="n">
-        <v>70.3</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1015,14 +1015,14 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Noruega</t>
+          <t>Eslováquia</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>69.90000000000001</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="C26" t="n">
-        <v>69.8</v>
+        <v>70.8</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1038,18 +1038,18 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Luxemburgo</t>
+          <t>Noruega</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>69.40000000000001</v>
+        <v>69.90000000000001</v>
       </c>
       <c r="C27" t="n">
-        <v>70.3</v>
+        <v>69.8</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1203,14 +1203,14 @@
         </is>
       </c>
       <c r="B34" t="n">
+        <v>66.40000000000001</v>
+      </c>
+      <c r="C34" t="n">
         <v>66.2</v>
       </c>
-      <c r="C34" t="n">
-        <v>66.40000000000001</v>
-      </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1226,14 +1226,14 @@
         </is>
       </c>
       <c r="B35" t="n">
+        <v>64.2</v>
+      </c>
+      <c r="C35" t="n">
         <v>64.09999999999999</v>
       </c>
-      <c r="C35" t="n">
-        <v>64.59999999999999</v>
-      </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2022-03</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">

</xml_diff>